<commit_message>
creación de logica front para consumo de la API usuario - organizador
</commit_message>
<xml_diff>
--- a/docs/plantilla_eventos.xlsx
+++ b/docs/plantilla_eventos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhona\OneDrive\Escritorio\Programacion\Proyectos\event-management-platform\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84424A8-4BB3-454C-A50E-09AD69C1C24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17399088-5C8E-4A12-8B67-4EA11486ECD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15720" xr2:uid="{900F8099-A353-4B59-B90F-BD9BD1F920ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>Bogotá</t>
   </si>
@@ -68,37 +68,37 @@
     <t>cupo_maximo</t>
   </si>
   <si>
-    <t>ExpoTech 2024</t>
-  </si>
-  <si>
-    <t>educativo</t>
-  </si>
-  <si>
     <t>presencial</t>
   </si>
   <si>
-    <t>Feria tecnológica</t>
-  </si>
-  <si>
-    <t>Calle 123 #45-67</t>
-  </si>
-  <si>
-    <t>Llevar cédula</t>
-  </si>
-  <si>
-    <t>Festival Arte</t>
-  </si>
-  <si>
-    <t>artístico</t>
-  </si>
-  <si>
-    <t>Música y pintura</t>
-  </si>
-  <si>
     <t>Cali</t>
   </si>
   <si>
-    <t>Cra 12 #34-56</t>
+    <t>Feria gastronomica</t>
+  </si>
+  <si>
+    <t>empresarial</t>
+  </si>
+  <si>
+    <t>Gastronomia de la región</t>
+  </si>
+  <si>
+    <t>parque principal</t>
+  </si>
+  <si>
+    <t>No aplican requisitos</t>
+  </si>
+  <si>
+    <t>Medellin</t>
+  </si>
+  <si>
+    <t>Ibague</t>
+  </si>
+  <si>
+    <t>Neiva</t>
+  </si>
+  <si>
+    <t>Barranquilla</t>
   </si>
 </sst>
 </file>
@@ -148,15 +148,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -167,18 +164,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,18 +502,16 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" style="4" customWidth="1"/>
-    <col min="4" max="6" width="18.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" style="3" customWidth="1"/>
+    <col min="4" max="8" width="18.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -550,262 +533,345 @@
       <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="D2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5">
+        <v>3118522588</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="5">
+        <v>3118522588</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5">
+        <v>3118522588</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3118522588</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="F6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="5">
+        <v>3118522588</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="C7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="7">
-        <v>3209582941</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="E7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="G7" s="5">
+        <v>3118522588</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="7">
-        <v>3119530072</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G7" s="9"/>
-      <c r="H7" s="5"/>
+      <c r="I7" s="5">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G8" s="9"/>
-      <c r="H8" s="5"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G9" s="9"/>
-      <c r="H9" s="5"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G10" s="9"/>
-      <c r="H10" s="5"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G11" s="9"/>
-      <c r="H11" s="5"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G12" s="9"/>
-      <c r="H12" s="5"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G13" s="9"/>
-      <c r="H13" s="5"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G14" s="9"/>
-      <c r="H14" s="5"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G15" s="9"/>
-      <c r="H15" s="5"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G16" s="9"/>
-      <c r="H16" s="5"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G17" s="9"/>
-      <c r="H17" s="5"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G18" s="9"/>
-      <c r="H18" s="5"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G19" s="9"/>
-      <c r="H19" s="5"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G20" s="9"/>
-      <c r="H20" s="5"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G21" s="9"/>
-      <c r="H21" s="5"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G22" s="9"/>
-      <c r="H22" s="5"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="4"/>
     </row>
     <row r="23" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G23" s="9"/>
-      <c r="H23" s="5"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G24" s="9"/>
-      <c r="H24" s="5"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="4"/>
     </row>
     <row r="25" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G25" s="9"/>
-      <c r="H25" s="5"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="4"/>
     </row>
     <row r="26" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G26" s="9"/>
-      <c r="H26" s="5"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="4"/>
     </row>
     <row r="27" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G27" s="9"/>
-      <c r="H27" s="5"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="4"/>
     </row>
     <row r="28" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G28" s="9"/>
-      <c r="H28" s="5"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="4"/>
     </row>
     <row r="29" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G29" s="9"/>
-      <c r="H29" s="5"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="4"/>
     </row>
     <row r="30" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G30" s="9"/>
-      <c r="H30" s="5"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="4"/>
     </row>
     <row r="31" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G31" s="9"/>
-      <c r="H31" s="5"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="4"/>
     </row>
     <row r="32" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G32" s="9"/>
-      <c r="H32" s="5"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="4"/>
     </row>
     <row r="33" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G33" s="9"/>
-      <c r="H33" s="5"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="4"/>
     </row>
     <row r="34" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G34" s="9"/>
-      <c r="H34" s="5"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="4"/>
     </row>
     <row r="35" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G35" s="9"/>
-      <c r="H35" s="5"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="4"/>
     </row>
     <row r="36" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G36" s="9"/>
-      <c r="H36" s="5"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="4"/>
     </row>
     <row r="37" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G37" s="9"/>
-      <c r="H37" s="5"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="4"/>
     </row>
     <row r="38" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G38" s="9"/>
-      <c r="H38" s="5"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="4"/>
     </row>
     <row r="39" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G39" s="9"/>
-      <c r="H39" s="5"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="4"/>
     </row>
     <row r="40" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G40" s="9"/>
-      <c r="H40" s="5"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="4"/>
     </row>
     <row r="41" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G41" s="9"/>
-      <c r="H41" s="5"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="4"/>
     </row>
     <row r="42" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G42" s="9"/>
-      <c r="H42" s="5"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="4"/>
     </row>
     <row r="43" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G43" s="9"/>
-      <c r="H43" s="5"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="4"/>
     </row>
     <row r="44" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G44" s="9"/>
-      <c r="H44" s="5"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="4"/>
     </row>
     <row r="45" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G45" s="9"/>
-      <c r="H45" s="5"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="4"/>
     </row>
     <row r="46" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G46" s="9"/>
-      <c r="H46" s="5"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Finalización de pruebas, plataforma operativa. Se inicia implementación de diseño en UX/UI
</commit_message>
<xml_diff>
--- a/docs/plantilla_eventos.xlsx
+++ b/docs/plantilla_eventos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhona\OneDrive\Escritorio\Programacion\Proyectos\event-management-platform\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17399088-5C8E-4A12-8B67-4EA11486ECD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC064DB-450D-4C81-8124-8F387D12300B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15720" xr2:uid="{900F8099-A353-4B59-B90F-BD9BD1F920ED}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
-  <si>
-    <t>Bogotá</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>nombre_evento</t>
   </si>
@@ -68,37 +65,25 @@
     <t>cupo_maximo</t>
   </si>
   <si>
-    <t>presencial</t>
-  </si>
-  <si>
-    <t>Cali</t>
-  </si>
-  <si>
-    <t>Feria gastronomica</t>
-  </si>
-  <si>
-    <t>empresarial</t>
-  </si>
-  <si>
-    <t>Gastronomia de la región</t>
-  </si>
-  <si>
-    <t>parque principal</t>
-  </si>
-  <si>
     <t>No aplican requisitos</t>
   </si>
   <si>
-    <t>Medellin</t>
-  </si>
-  <si>
-    <t>Ibague</t>
-  </si>
-  <si>
-    <t>Neiva</t>
-  </si>
-  <si>
-    <t>Barranquilla</t>
+    <t>artístico</t>
+  </si>
+  <si>
+    <t>virtual</t>
+  </si>
+  <si>
+    <t>Clase gastronomica</t>
+  </si>
+  <si>
+    <t>Gastronomia virtual</t>
+  </si>
+  <si>
+    <t>no aplica</t>
+  </si>
+  <si>
+    <t>Clase astronomica</t>
   </si>
 </sst>
 </file>
@@ -499,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583070D7-D636-42C1-BCCB-445B0CAF9457}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,31 +501,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -548,174 +533,95 @@
         <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>0</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G2" s="5">
-        <v>3118522588</v>
+        <v>3118522584</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="I2" s="5">
-        <v>40</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="F3" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G3" s="5">
-        <v>3118522588</v>
+        <v>3118522584</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="I3" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="5">
-        <v>3118522588</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="5">
-        <v>3118522588</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="5">
-        <v>3118522588</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="5">
-        <v>3118522588</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="5">
-        <v>40</v>
-      </c>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" s="1"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G8" s="1"/>
@@ -868,10 +774,6 @@
     <row r="45" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G45" s="1"/>
       <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G46" s="1"/>
-      <c r="H46" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
test carga masiva eventos
</commit_message>
<xml_diff>
--- a/docs/plantilla_eventos.xlsx
+++ b/docs/plantilla_eventos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhona\OneDrive\Escritorio\Programacion\Proyectos\event-management-platform\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC064DB-450D-4C81-8124-8F387D12300B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180EA7AA-BE98-483A-B120-6E0BD2E085A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15720" xr2:uid="{900F8099-A353-4B59-B90F-BD9BD1F920ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>nombre_evento</t>
   </si>
@@ -68,22 +68,40 @@
     <t>No aplican requisitos</t>
   </si>
   <si>
-    <t>artístico</t>
-  </si>
-  <si>
     <t>virtual</t>
   </si>
   <si>
-    <t>Clase gastronomica</t>
-  </si>
-  <si>
-    <t>Gastronomia virtual</t>
-  </si>
-  <si>
     <t>no aplica</t>
   </si>
   <si>
-    <t>Clase astronomica</t>
+    <t>Clase 1</t>
+  </si>
+  <si>
+    <t>empresarial</t>
+  </si>
+  <si>
+    <t>deportivo</t>
+  </si>
+  <si>
+    <t>presencial</t>
+  </si>
+  <si>
+    <t>clase 1 1 1 1 1</t>
+  </si>
+  <si>
+    <t>clase 2 2 2 2 2</t>
+  </si>
+  <si>
+    <t>Barranquilla</t>
+  </si>
+  <si>
+    <t>url//</t>
+  </si>
+  <si>
+    <t>dg 59 # 45-65</t>
+  </si>
+  <si>
+    <t>internet y equipo</t>
   </si>
 </sst>
 </file>
@@ -487,7 +505,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,57 +551,57 @@
         <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G2" s="5">
-        <v>3118522584</v>
+        <v>3118522123</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="I2" s="5">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G3" s="5">
-        <v>3118522584</v>
+        <v>3118522123</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="I3" s="5">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>